<commit_message>
create score transUnion Author: DEFAULT. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/ExternalSources/Main.xlsx
+++ b/DESIGN/rules/ExternalSources/Main.xlsx
@@ -13,23 +13,359 @@
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+  <si>
+    <t>SimpleRules DoubleValue ScoreTransUnion(String id)</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>RETURN</t>
+  </si>
+  <si>
+    <t>1023881928</t>
+  </si>
+  <si>
+    <t>87</t>
+  </si>
+  <si>
+    <t>1010228244</t>
+  </si>
+  <si>
+    <t>98</t>
+  </si>
+  <si>
+    <t>1024510404</t>
+  </si>
+  <si>
+    <t>76</t>
+  </si>
+  <si>
+    <t>1023881999</t>
+  </si>
+  <si>
+    <t>56</t>
+  </si>
+  <si>
+    <t>1010228299</t>
+  </si>
+  <si>
+    <t>102</t>
+  </si>
+  <si>
+    <t>1024510499</t>
+  </si>
+  <si>
+    <t>97</t>
+  </si>
+  <si>
+    <t>1023881988</t>
+  </si>
+  <si>
+    <t>23</t>
+  </si>
+  <si>
+    <t>1010228288</t>
+  </si>
+  <si>
+    <t>1024510488</t>
+  </si>
+  <si>
+    <t>1023881977</t>
+  </si>
+  <si>
+    <t>43</t>
+  </si>
+  <si>
+    <t>1010228277</t>
+  </si>
+  <si>
+    <t>1024510477</t>
+  </si>
+  <si>
+    <t>27</t>
+  </si>
+  <si>
+    <t>1023881966</t>
+  </si>
+  <si>
+    <t>78</t>
+  </si>
+  <si>
+    <t>1010228266</t>
+  </si>
+  <si>
+    <t>28</t>
+  </si>
+  <si>
+    <t>1024510466</t>
+  </si>
+  <si>
+    <t>34</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="0"/>
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
     </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <b val="true"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color indexed="8"/>
+      <u val="none"/>
+    </font>
+    <font>
+      <name val="&quot;Franklin Gothik Book&quot;"/>
+      <sz val="10.0"/>
+      <color rgb="000001"/>
+      <u val="none"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="A6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="A6A6A6"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FAD246"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FAD246"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="FFFFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="none">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="D9D9D9"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -37,11 +373,576 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <top>
+        <color rgb="000000"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000000"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="DDDDDD"/>
+      </bottom>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top>
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right>
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom>
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="DDDDDD"/>
+      </left>
+      <right style="thin">
+        <color rgb="DDDDDD"/>
+      </right>
+      <top style="thin">
+        <color rgb="DDDDDD"/>
+      </top>
+      <bottom style="thick">
+        <color rgb="FFC91D"/>
+      </bottom>
+    </border>
+    <border>
+      <top>
+        <color rgb="000001"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+    </border>
+    <border>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top>
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <right>
+        <color rgb="000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom>
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <left>
+        <color rgb="000000"/>
+      </left>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
+    <border>
+      <top style="thin">
+        <color rgb="000001"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="000001"/>
+      </bottom>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="35">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="14" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="7" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="9" borderId="22" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="7" borderId="28" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="9" borderId="34" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="7" borderId="42" xfId="0" applyFill="true" applyBorder="true" applyFont="true">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
@@ -344,12 +1245,150 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="B3:C19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="125" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <sheetData>
+    <row r="3">
+      <c r="B3" s="33" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="33"/>
+    </row>
+    <row r="4">
+      <c r="B4" t="s" s="1">
+        <v>1</v>
+      </c>
+      <c r="C4" t="s" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="B5" t="s" s="3">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s" s="4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="B6" t="s" s="5">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s" s="6">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="B7" t="s" s="7">
+        <v>7</v>
+      </c>
+      <c r="C7" t="s" s="8">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="B8" t="s" s="9">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s" s="10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="9">
+      <c r="B9" t="s" s="11">
+        <v>11</v>
+      </c>
+      <c r="C9" t="s" s="12">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="10">
+      <c r="B10" t="s" s="13">
+        <v>13</v>
+      </c>
+      <c r="C10" t="s" s="14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11">
+      <c r="B11" t="s" s="15">
+        <v>15</v>
+      </c>
+      <c r="C11" t="s" s="16">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="B12" t="s" s="17">
+        <v>17</v>
+      </c>
+      <c r="C12" t="s" s="18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="B13" t="s" s="19">
+        <v>18</v>
+      </c>
+      <c r="C13" t="s" s="20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="B14" t="s" s="21">
+        <v>19</v>
+      </c>
+      <c r="C14" t="s" s="22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="B15" t="s" s="23">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s" s="24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="B16" t="s" s="25">
+        <v>22</v>
+      </c>
+      <c r="C16" t="s" s="26">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="B17" t="s" s="27">
+        <v>24</v>
+      </c>
+      <c r="C17" t="s" s="28">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="B18" t="s" s="29">
+        <v>26</v>
+      </c>
+      <c r="C18" t="s" s="30">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="B19" t="s" s="31">
+        <v>28</v>
+      </c>
+      <c r="C19" t="s" s="32">
+        <v>29</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B3:C3"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>